<commit_message>
single and scene simulations and analyzes with Wheat-BRIDGES
</commit_message>
<xml_diff>
--- a/simulations/scene/inputs/Scenarios_25-06-05.xlsx
+++ b/simulations/scene/inputs/Scenarios_25-06-05.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp00839\home\torisuten\package\Wheat-BRIDGES\simulations\scene\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp42424\home\torisuten\package\Wheat-BRIDGES\simulations\scene\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E55B8CA-F23A-4335-9763-706995C8E265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97525875-1336-4A82-B4BC-3D31B3D19FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2877,10 +2877,10 @@
   <dimension ref="A1:BZ229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="O192" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="N192" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S231" sqref="S231"/>
+      <selection pane="bottomRight" activeCell="R206" sqref="R206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33163,8 +33163,8 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="R205" s="44">
-        <f>0.00005 / 100 *10</f>
-        <v>4.9999999999999996E-6</v>
+        <f>0.00005 / 100 / 6</f>
+        <v>8.3333333333333325E-8</v>
       </c>
       <c r="S205" s="44">
         <f>0.00005 / 100</f>

</xml_diff>